<commit_message>
xong xuat view bac ai
</commit_message>
<xml_diff>
--- a/public/export/giaidoan.dahuoai.xlsx
+++ b/public/export/giaidoan.dahuoai.xlsx
@@ -2746,19 +2746,19 @@
       </c>
       <c r="E6" s="8">
         <f>E7+E14+E17</f>
-        <v>0</v>
+        <v>119.9</v>
       </c>
       <c r="F6" s="8">
         <f>F7+F14+F17</f>
-        <v>0</v>
+        <v>124</v>
       </c>
       <c r="G6" s="8">
         <f>G7+G14+G17</f>
-        <v>0</v>
+        <v>129.1</v>
       </c>
       <c r="H6" s="8">
         <f>H7+H14+H17</f>
-        <v>0</v>
+        <v>134</v>
       </c>
       <c r="I6" s="22">
         <f>I7+I14+I17</f>
@@ -2770,11 +2770,11 @@
       </c>
       <c r="K6" s="29">
         <f>K7+K14+K17</f>
-        <v>0</v>
+        <v>169.6</v>
       </c>
       <c r="L6" s="30">
         <f>L7+L14+L17</f>
-        <v>0</v>
+        <v>170.8</v>
       </c>
       <c r="M6" s="38">
         <f>M7+M14+M17</f>
@@ -2849,7 +2849,7 @@
       <c r="BM6" s="38"/>
       <c r="BN6" s="38"/>
       <c r="BO6" s="38"/>
-      <c r="BP6" s="38" t="str">
+      <c r="BP6" s="38">
         <f>(J6/E6)^(1/5)*100</f>
         <v>0</v>
       </c>
@@ -2859,7 +2859,7 @@
       </c>
       <c r="BR6" s="38">
         <f>J6-E6</f>
-        <v>0</v>
+        <v>-119.9</v>
       </c>
       <c r="BS6" s="38">
         <f>P6-J6</f>
@@ -2869,7 +2869,7 @@
         <f>J6/I6*100</f>
         <v>0</v>
       </c>
-      <c r="BU6" s="29" t="str">
+      <c r="BU6" s="29">
         <f>J6/K6*100</f>
         <v>0</v>
       </c>
@@ -4333,19 +4333,19 @@
       </c>
       <c r="E17" s="8">
         <f>Q179</f>
-        <v>0</v>
+        <v>119.9</v>
       </c>
       <c r="F17" s="8">
         <f>R179</f>
-        <v>0</v>
+        <v>124</v>
       </c>
       <c r="G17" s="8">
         <f>S179</f>
-        <v>0</v>
+        <v>129.1</v>
       </c>
       <c r="H17" s="8">
         <f>T179</f>
-        <v>0</v>
+        <v>134</v>
       </c>
       <c r="I17" s="22">
         <f>U179</f>
@@ -4357,11 +4357,11 @@
       </c>
       <c r="K17" s="29">
         <f>W179</f>
-        <v>0</v>
+        <v>169.6</v>
       </c>
       <c r="L17" s="30">
         <f>X179</f>
-        <v>0</v>
+        <v>170.8</v>
       </c>
       <c r="M17" s="38">
         <f>Y179</f>
@@ -4436,7 +4436,7 @@
       <c r="BM17" s="38"/>
       <c r="BN17" s="38"/>
       <c r="BO17" s="38"/>
-      <c r="BP17" s="38" t="str">
+      <c r="BP17" s="38">
         <f>(J17/E17)^(1/5)*100</f>
         <v>0</v>
       </c>
@@ -4446,7 +4446,7 @@
       </c>
       <c r="BR17" s="38">
         <f>J17-E17</f>
-        <v>0</v>
+        <v>-119.9</v>
       </c>
       <c r="BS17" s="38">
         <f>P17-J17</f>
@@ -4456,7 +4456,7 @@
         <f>J17/I17*100</f>
         <v>0</v>
       </c>
-      <c r="BU17" s="29" t="str">
+      <c r="BU17" s="29">
         <f>J17/K17*100</f>
         <v>0</v>
       </c>
@@ -4480,19 +4480,19 @@
       </c>
       <c r="E18" s="8">
         <f>E19+E26+E29</f>
-        <v>0</v>
+        <v>18.5</v>
       </c>
       <c r="F18" s="8">
         <f>F19+F26+F29</f>
-        <v>0</v>
+        <v>17.9</v>
       </c>
       <c r="G18" s="8">
         <f>G19+G26+G29</f>
-        <v>0</v>
+        <v>18.6</v>
       </c>
       <c r="H18" s="8">
         <f>H19+H26+H29</f>
-        <v>0</v>
+        <v>24.3</v>
       </c>
       <c r="I18" s="22">
         <f>I19+I26+I29</f>
@@ -4504,11 +4504,11 @@
       </c>
       <c r="K18" s="29">
         <f>K19+K26+K29</f>
-        <v>0</v>
+        <v>26.6</v>
       </c>
       <c r="L18" s="30">
         <f>L19+L26+L29</f>
-        <v>0</v>
+        <v>27.7</v>
       </c>
       <c r="M18" s="38">
         <f>M19+M26+M29</f>
@@ -4583,7 +4583,7 @@
       <c r="BM18" s="38"/>
       <c r="BN18" s="38"/>
       <c r="BO18" s="38"/>
-      <c r="BP18" s="38" t="str">
+      <c r="BP18" s="38">
         <f>(J18/E18)^(1/5)*100</f>
         <v>0</v>
       </c>
@@ -4593,7 +4593,7 @@
       </c>
       <c r="BR18" s="38">
         <f>J18-E18</f>
-        <v>0</v>
+        <v>-18.5</v>
       </c>
       <c r="BS18" s="38">
         <f>P18-J18</f>
@@ -4603,7 +4603,7 @@
         <f>J18/I18*100</f>
         <v>0</v>
       </c>
-      <c r="BU18" s="29" t="str">
+      <c r="BU18" s="29">
         <f>J18/K18*100</f>
         <v>0</v>
       </c>
@@ -6067,19 +6067,19 @@
       </c>
       <c r="E29" s="8">
         <f>Q195</f>
-        <v>0</v>
+        <v>18.5</v>
       </c>
       <c r="F29" s="8">
         <f>R195</f>
-        <v>0</v>
+        <v>17.9</v>
       </c>
       <c r="G29" s="8">
         <f>S195</f>
-        <v>0</v>
+        <v>18.6</v>
       </c>
       <c r="H29" s="8">
         <f>T195</f>
-        <v>0</v>
+        <v>24.3</v>
       </c>
       <c r="I29" s="22">
         <f>U195</f>
@@ -6091,11 +6091,11 @@
       </c>
       <c r="K29" s="29">
         <f>W195</f>
-        <v>0</v>
+        <v>26.6</v>
       </c>
       <c r="L29" s="30">
         <f>X195</f>
-        <v>0</v>
+        <v>27.7</v>
       </c>
       <c r="M29" s="38">
         <f>Y195</f>
@@ -6170,7 +6170,7 @@
       <c r="BM29" s="38"/>
       <c r="BN29" s="38"/>
       <c r="BO29" s="38"/>
-      <c r="BP29" s="38" t="str">
+      <c r="BP29" s="38">
         <f>(J29/E29)^(1/5)*100</f>
         <v>0</v>
       </c>
@@ -6180,7 +6180,7 @@
       </c>
       <c r="BR29" s="38">
         <f>J29-E29</f>
-        <v>0</v>
+        <v>-18.5</v>
       </c>
       <c r="BS29" s="38">
         <f>P29-J29</f>
@@ -6190,7 +6190,7 @@
         <f>J29/I29*100</f>
         <v>0</v>
       </c>
-      <c r="BU29" s="29" t="str">
+      <c r="BU29" s="29">
         <f>J29/K29*100</f>
         <v>0</v>
       </c>
@@ -6214,19 +6214,19 @@
       </c>
       <c r="E30" s="8">
         <f>E31+E32+E33</f>
-        <v>0</v>
+        <v>13.135</v>
       </c>
       <c r="F30" s="8">
         <f>F31+F32+F33</f>
-        <v>0</v>
+        <v>12.709</v>
       </c>
       <c r="G30" s="8">
         <f>G31+G32+G33</f>
-        <v>0</v>
+        <v>13.206</v>
       </c>
       <c r="H30" s="8">
         <f>H31+H32+H33</f>
-        <v>0</v>
+        <v>17.253</v>
       </c>
       <c r="I30" s="22">
         <f>I31+I32+I33</f>
@@ -6238,11 +6238,11 @@
       </c>
       <c r="K30" s="29">
         <f>K31+K32+K33</f>
-        <v>0</v>
+        <v>18.886</v>
       </c>
       <c r="L30" s="30">
         <f>L31+L32+L33</f>
-        <v>0</v>
+        <v>19.667</v>
       </c>
       <c r="M30" s="38">
         <f>M31+M32+M33</f>
@@ -6317,7 +6317,7 @@
       <c r="BM30" s="38"/>
       <c r="BN30" s="38"/>
       <c r="BO30" s="38"/>
-      <c r="BP30" s="38" t="str">
+      <c r="BP30" s="38">
         <f>(J30/E30)^(1/5)*100</f>
         <v>0</v>
       </c>
@@ -6327,7 +6327,7 @@
       </c>
       <c r="BR30" s="38">
         <f>J30-E30</f>
-        <v>0</v>
+        <v>-13.135</v>
       </c>
       <c r="BS30" s="38">
         <f>P30-J30</f>
@@ -6337,7 +6337,7 @@
         <f>J30/I30*100</f>
         <v>0</v>
       </c>
-      <c r="BU30" s="29" t="str">
+      <c r="BU30" s="29">
         <f>J30/K30*100</f>
         <v>0</v>
       </c>
@@ -6649,19 +6649,19 @@
       </c>
       <c r="E33" s="8">
         <f>E29*0.71</f>
-        <v>0</v>
+        <v>13.135</v>
       </c>
       <c r="F33" s="8">
         <f>F29*0.71</f>
-        <v>0</v>
+        <v>12.709</v>
       </c>
       <c r="G33" s="8">
         <f>G29*0.71</f>
-        <v>0</v>
+        <v>13.206</v>
       </c>
       <c r="H33" s="8">
         <f>H29*0.71</f>
-        <v>0</v>
+        <v>17.253</v>
       </c>
       <c r="I33" s="22">
         <f>I29*0.71</f>
@@ -6673,11 +6673,11 @@
       </c>
       <c r="K33" s="29">
         <f>K29*0.71</f>
-        <v>0</v>
+        <v>18.886</v>
       </c>
       <c r="L33" s="30">
         <f>L29*0.71</f>
-        <v>0</v>
+        <v>19.667</v>
       </c>
       <c r="M33" s="38">
         <f>M29*0.71</f>
@@ -6752,7 +6752,7 @@
       <c r="BM33" s="38"/>
       <c r="BN33" s="38"/>
       <c r="BO33" s="38"/>
-      <c r="BP33" s="38" t="str">
+      <c r="BP33" s="38">
         <f>(J33/E33)^(1/5)*100</f>
         <v>0</v>
       </c>
@@ -6762,7 +6762,7 @@
       </c>
       <c r="BR33" s="38">
         <f>J33-E33</f>
-        <v>0</v>
+        <v>-13.135</v>
       </c>
       <c r="BS33" s="38">
         <f>P33-J33</f>
@@ -6772,7 +6772,7 @@
         <f>J33/I33*100</f>
         <v>0</v>
       </c>
-      <c r="BU33" s="29" t="str">
+      <c r="BU33" s="29">
         <f>J33/K33*100</f>
         <v>0</v>
       </c>
@@ -6794,21 +6794,21 @@
       <c r="D34" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="E34" s="8" t="str">
+      <c r="E34" s="8">
         <f>E35+E36+E37</f>
-        <v>0</v>
-      </c>
-      <c r="F34" s="8" t="str">
+        <v>100</v>
+      </c>
+      <c r="F34" s="8">
         <f>F35+F36+F37</f>
-        <v>0</v>
-      </c>
-      <c r="G34" s="8" t="str">
+        <v>100</v>
+      </c>
+      <c r="G34" s="8">
         <f>G35+G36+G37</f>
-        <v>0</v>
-      </c>
-      <c r="H34" s="8" t="str">
+        <v>100</v>
+      </c>
+      <c r="H34" s="8">
         <f>H35+H36+H37</f>
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="I34" s="22" t="str">
         <f>I35+I36+I37</f>
@@ -6818,13 +6818,13 @@
         <f>J35+J36+J37</f>
         <v>0</v>
       </c>
-      <c r="K34" s="29" t="str">
+      <c r="K34" s="29">
         <f>K35+K36+K37</f>
-        <v>0</v>
-      </c>
-      <c r="L34" s="30" t="str">
+        <v>100</v>
+      </c>
+      <c r="L34" s="30">
         <f>L35+L36+L37</f>
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="M34" s="38" t="str">
         <f>M35+M36+M37</f>
@@ -6939,19 +6939,19 @@
       <c r="D35" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="E35" s="8" t="str">
+      <c r="E35" s="8">
         <f>E31/E30*100</f>
         <v>0</v>
       </c>
-      <c r="F35" s="8" t="str">
+      <c r="F35" s="8">
         <f>F31/F30*100</f>
         <v>0</v>
       </c>
-      <c r="G35" s="8" t="str">
+      <c r="G35" s="8">
         <f>G31/G30*100</f>
         <v>0</v>
       </c>
-      <c r="H35" s="8" t="str">
+      <c r="H35" s="8">
         <f>H31/H30*100</f>
         <v>0</v>
       </c>
@@ -6963,11 +6963,11 @@
         <f>J31/J30*100</f>
         <v>0</v>
       </c>
-      <c r="K35" s="29" t="str">
+      <c r="K35" s="29">
         <f>K31/K30*100</f>
         <v>0</v>
       </c>
-      <c r="L35" s="30" t="str">
+      <c r="L35" s="30">
         <f>L31/L30*100</f>
         <v>0</v>
       </c>
@@ -7084,19 +7084,19 @@
       <c r="D36" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="E36" s="8" t="str">
+      <c r="E36" s="8">
         <f>E32/E30*100</f>
         <v>0</v>
       </c>
-      <c r="F36" s="8" t="str">
+      <c r="F36" s="8">
         <f>F32/F30*100</f>
         <v>0</v>
       </c>
-      <c r="G36" s="8" t="str">
+      <c r="G36" s="8">
         <f>G32/G30*100</f>
         <v>0</v>
       </c>
-      <c r="H36" s="8" t="str">
+      <c r="H36" s="8">
         <f>H32/H30*100</f>
         <v>0</v>
       </c>
@@ -7108,11 +7108,11 @@
         <f>J32/J30*100</f>
         <v>0</v>
       </c>
-      <c r="K36" s="29" t="str">
+      <c r="K36" s="29">
         <f>K32/K30*100</f>
         <v>0</v>
       </c>
-      <c r="L36" s="30" t="str">
+      <c r="L36" s="30">
         <f>L32/L30*100</f>
         <v>0</v>
       </c>
@@ -7229,21 +7229,21 @@
       <c r="D37" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="E37" s="8" t="str">
+      <c r="E37" s="8">
         <f>E33/E30*100</f>
-        <v>0</v>
-      </c>
-      <c r="F37" s="8" t="str">
+        <v>100</v>
+      </c>
+      <c r="F37" s="8">
         <f>F33/F30*100</f>
-        <v>0</v>
-      </c>
-      <c r="G37" s="8" t="str">
+        <v>100</v>
+      </c>
+      <c r="G37" s="8">
         <f>G33/G30*100</f>
-        <v>0</v>
-      </c>
-      <c r="H37" s="8" t="str">
+        <v>100</v>
+      </c>
+      <c r="H37" s="8">
         <f>H33/H30*100</f>
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="I37" s="22" t="str">
         <f>I33/I30*100</f>
@@ -7253,13 +7253,13 @@
         <f>J33/J30*100</f>
         <v>0</v>
       </c>
-      <c r="K37" s="29" t="str">
+      <c r="K37" s="29">
         <f>K33/K30*100</f>
-        <v>0</v>
-      </c>
-      <c r="L37" s="30" t="str">
+        <v>100</v>
+      </c>
+      <c r="L37" s="30">
         <f>L33/L30*100</f>
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="M37" s="38" t="str">
         <f>M33/M30*100</f>
@@ -7670,11 +7670,11 @@
         <f>J36/J33*100</f>
         <v>0</v>
       </c>
-      <c r="K40" s="76" t="str">
+      <c r="K40" s="76">
         <f>K36/K33*100</f>
         <v>0</v>
       </c>
-      <c r="L40" s="77" t="str">
+      <c r="L40" s="77">
         <f>L36/L33*100</f>
         <v>0</v>
       </c>
@@ -7793,13 +7793,13 @@
         <f>J37/J34*100</f>
         <v>0</v>
       </c>
-      <c r="K41" s="53" t="str">
+      <c r="K41" s="53">
         <f>K37/K34*100</f>
-        <v>0</v>
-      </c>
-      <c r="L41" s="37" t="str">
+        <v>100</v>
+      </c>
+      <c r="L41" s="37">
         <f>L37/L34*100</f>
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="M41" s="66"/>
       <c r="N41" s="66"/>
@@ -8200,11 +8200,11 @@
         <f>J40/J37*100</f>
         <v>0</v>
       </c>
-      <c r="K44" s="52" t="str">
+      <c r="K44" s="52">
         <f>K40/K37*100</f>
         <v>0</v>
       </c>
-      <c r="L44" s="62" t="str">
+      <c r="L44" s="62">
         <f>L40/L37*100</f>
         <v>0</v>
       </c>
@@ -9084,11 +9084,11 @@
         <f>J44/J41*100</f>
         <v>0</v>
       </c>
-      <c r="K48" s="52" t="str">
+      <c r="K48" s="52">
         <f>K44/K41*100</f>
         <v>0</v>
       </c>
-      <c r="L48" s="62" t="str">
+      <c r="L48" s="62">
         <f>L44/L41*100</f>
         <v>0</v>
       </c>
@@ -38991,16 +38991,16 @@
       <c r="O178" s="52"/>
       <c r="P178" s="52"/>
       <c r="Q178" s="52">
-        <v>0</v>
+        <v>135.5</v>
       </c>
       <c r="R178" s="52">
-        <v>0</v>
+        <v>146.9</v>
       </c>
       <c r="S178" s="52">
-        <v>0</v>
+        <v>160.9</v>
       </c>
       <c r="T178" s="52">
-        <v>0</v>
+        <v>171.2</v>
       </c>
       <c r="U178" s="52">
         <v>0</v>
@@ -39009,10 +39009,10 @@
         <v>0</v>
       </c>
       <c r="W178" s="52">
-        <v>0</v>
+        <v>195.2</v>
       </c>
       <c r="X178" s="52">
-        <v>0</v>
+        <v>207.4</v>
       </c>
       <c r="Y178" s="52">
         <v>0</v>
@@ -39247,16 +39247,16 @@
         <v>0</v>
       </c>
       <c r="Q179" s="52">
-        <v>0</v>
+        <v>119.9</v>
       </c>
       <c r="R179" s="52">
-        <v>0</v>
+        <v>124</v>
       </c>
       <c r="S179" s="52">
-        <v>0</v>
+        <v>129.1</v>
       </c>
       <c r="T179" s="52">
-        <v>0</v>
+        <v>134</v>
       </c>
       <c r="U179" s="52">
         <v>0</v>
@@ -39265,10 +39265,10 @@
         <v>0</v>
       </c>
       <c r="W179" s="52">
-        <v>0</v>
+        <v>169.6</v>
       </c>
       <c r="X179" s="52">
-        <v>0</v>
+        <v>170.8</v>
       </c>
       <c r="Y179" s="52">
         <v>0</v>
@@ -39480,31 +39480,81 @@
       <c r="N180" s="58"/>
       <c r="O180" s="58"/>
       <c r="P180" s="58"/>
-      <c r="Q180" s="58"/>
-      <c r="R180" s="58"/>
-      <c r="S180" s="58"/>
-      <c r="T180" s="58"/>
-      <c r="U180" s="58"/>
-      <c r="V180" s="58"/>
-      <c r="W180" s="58"/>
-      <c r="X180" s="58"/>
-      <c r="Y180" s="58"/>
-      <c r="Z180" s="58"/>
-      <c r="AA180" s="58"/>
-      <c r="AB180" s="58"/>
-      <c r="AC180" s="52"/>
-      <c r="AD180" s="59"/>
-      <c r="AE180" s="59"/>
-      <c r="AF180" s="59"/>
-      <c r="AG180" s="59"/>
-      <c r="AH180" s="59"/>
-      <c r="AI180" s="59"/>
-      <c r="AJ180" s="59"/>
-      <c r="AK180" s="59"/>
-      <c r="AL180" s="59"/>
-      <c r="AM180" s="59"/>
-      <c r="AN180" s="59"/>
-      <c r="AO180" s="59"/>
+      <c r="Q180" s="58">
+        <v>13.7</v>
+      </c>
+      <c r="R180" s="58">
+        <v>13.8</v>
+      </c>
+      <c r="S180" s="58">
+        <v>13.9</v>
+      </c>
+      <c r="T180" s="58">
+        <v>14</v>
+      </c>
+      <c r="U180" s="58">
+        <v>0</v>
+      </c>
+      <c r="V180" s="58">
+        <v>0</v>
+      </c>
+      <c r="W180" s="58">
+        <v>15.5</v>
+      </c>
+      <c r="X180" s="58">
+        <v>15.7</v>
+      </c>
+      <c r="Y180" s="58">
+        <v>0</v>
+      </c>
+      <c r="Z180" s="58">
+        <v>0</v>
+      </c>
+      <c r="AA180" s="58">
+        <v>0</v>
+      </c>
+      <c r="AB180" s="58">
+        <v>0</v>
+      </c>
+      <c r="AC180" s="52">
+        <v>0</v>
+      </c>
+      <c r="AD180" s="59">
+        <v>0</v>
+      </c>
+      <c r="AE180" s="59">
+        <v>0</v>
+      </c>
+      <c r="AF180" s="59">
+        <v>0</v>
+      </c>
+      <c r="AG180" s="59">
+        <v>0</v>
+      </c>
+      <c r="AH180" s="59">
+        <v>0</v>
+      </c>
+      <c r="AI180" s="59">
+        <v>0</v>
+      </c>
+      <c r="AJ180" s="59">
+        <v>0</v>
+      </c>
+      <c r="AK180" s="59">
+        <v>0</v>
+      </c>
+      <c r="AL180" s="59">
+        <v>0</v>
+      </c>
+      <c r="AM180" s="59">
+        <v>0</v>
+      </c>
+      <c r="AN180" s="59">
+        <v>0</v>
+      </c>
+      <c r="AO180" s="59">
+        <v>0</v>
+      </c>
       <c r="AP180" s="58">
         <f>Q180*AC180/1000000000</f>
         <v>0</v>
@@ -39664,31 +39714,81 @@
       <c r="N181" s="58"/>
       <c r="O181" s="58"/>
       <c r="P181" s="58"/>
-      <c r="Q181" s="58"/>
-      <c r="R181" s="58"/>
-      <c r="S181" s="58"/>
-      <c r="T181" s="58"/>
-      <c r="U181" s="58"/>
-      <c r="V181" s="58"/>
-      <c r="W181" s="58"/>
-      <c r="X181" s="58"/>
-      <c r="Y181" s="58"/>
-      <c r="Z181" s="58"/>
-      <c r="AA181" s="58"/>
-      <c r="AB181" s="58"/>
-      <c r="AC181" s="52"/>
-      <c r="AD181" s="59"/>
-      <c r="AE181" s="59"/>
-      <c r="AF181" s="59"/>
-      <c r="AG181" s="59"/>
-      <c r="AH181" s="59"/>
-      <c r="AI181" s="59"/>
-      <c r="AJ181" s="59"/>
-      <c r="AK181" s="59"/>
-      <c r="AL181" s="59"/>
-      <c r="AM181" s="59"/>
-      <c r="AN181" s="59"/>
-      <c r="AO181" s="59"/>
+      <c r="Q181" s="58">
+        <v>26.1</v>
+      </c>
+      <c r="R181" s="58">
+        <v>28.5</v>
+      </c>
+      <c r="S181" s="58">
+        <v>31.2</v>
+      </c>
+      <c r="T181" s="58">
+        <v>35.6</v>
+      </c>
+      <c r="U181" s="58">
+        <v>0</v>
+      </c>
+      <c r="V181" s="58">
+        <v>0</v>
+      </c>
+      <c r="W181" s="58">
+        <v>45.9</v>
+      </c>
+      <c r="X181" s="58">
+        <v>51.4</v>
+      </c>
+      <c r="Y181" s="58">
+        <v>0</v>
+      </c>
+      <c r="Z181" s="58">
+        <v>0</v>
+      </c>
+      <c r="AA181" s="58">
+        <v>0</v>
+      </c>
+      <c r="AB181" s="58">
+        <v>0</v>
+      </c>
+      <c r="AC181" s="52">
+        <v>0</v>
+      </c>
+      <c r="AD181" s="59">
+        <v>0</v>
+      </c>
+      <c r="AE181" s="59">
+        <v>0</v>
+      </c>
+      <c r="AF181" s="59">
+        <v>0</v>
+      </c>
+      <c r="AG181" s="59">
+        <v>0</v>
+      </c>
+      <c r="AH181" s="59">
+        <v>0</v>
+      </c>
+      <c r="AI181" s="59">
+        <v>0</v>
+      </c>
+      <c r="AJ181" s="59">
+        <v>0</v>
+      </c>
+      <c r="AK181" s="59">
+        <v>0</v>
+      </c>
+      <c r="AL181" s="59">
+        <v>0</v>
+      </c>
+      <c r="AM181" s="59">
+        <v>0</v>
+      </c>
+      <c r="AN181" s="59">
+        <v>0</v>
+      </c>
+      <c r="AO181" s="59">
+        <v>0</v>
+      </c>
       <c r="AP181" s="58">
         <f>Q181*AC181/1000000000</f>
         <v>0</v>
@@ -39848,31 +39948,81 @@
       <c r="N182" s="58"/>
       <c r="O182" s="58"/>
       <c r="P182" s="58"/>
-      <c r="Q182" s="58"/>
-      <c r="R182" s="58"/>
-      <c r="S182" s="58"/>
-      <c r="T182" s="58"/>
-      <c r="U182" s="58"/>
-      <c r="V182" s="58"/>
-      <c r="W182" s="58"/>
-      <c r="X182" s="58"/>
-      <c r="Y182" s="58"/>
-      <c r="Z182" s="58"/>
-      <c r="AA182" s="58"/>
-      <c r="AB182" s="58"/>
-      <c r="AC182" s="52"/>
-      <c r="AD182" s="59"/>
-      <c r="AE182" s="59"/>
-      <c r="AF182" s="59"/>
-      <c r="AG182" s="59"/>
-      <c r="AH182" s="59"/>
-      <c r="AI182" s="59"/>
-      <c r="AJ182" s="59"/>
-      <c r="AK182" s="59"/>
-      <c r="AL182" s="59"/>
-      <c r="AM182" s="59"/>
-      <c r="AN182" s="59"/>
-      <c r="AO182" s="59"/>
+      <c r="Q182" s="58">
+        <v>0.9</v>
+      </c>
+      <c r="R182" s="58">
+        <v>0.9</v>
+      </c>
+      <c r="S182" s="58">
+        <v>1</v>
+      </c>
+      <c r="T182" s="58">
+        <v>1</v>
+      </c>
+      <c r="U182" s="58">
+        <v>0</v>
+      </c>
+      <c r="V182" s="58">
+        <v>0</v>
+      </c>
+      <c r="W182" s="58">
+        <v>1.3</v>
+      </c>
+      <c r="X182" s="58">
+        <v>1.3</v>
+      </c>
+      <c r="Y182" s="58">
+        <v>0</v>
+      </c>
+      <c r="Z182" s="58">
+        <v>0</v>
+      </c>
+      <c r="AA182" s="58">
+        <v>0</v>
+      </c>
+      <c r="AB182" s="58">
+        <v>0</v>
+      </c>
+      <c r="AC182" s="52">
+        <v>0</v>
+      </c>
+      <c r="AD182" s="59">
+        <v>0</v>
+      </c>
+      <c r="AE182" s="59">
+        <v>0</v>
+      </c>
+      <c r="AF182" s="59">
+        <v>0</v>
+      </c>
+      <c r="AG182" s="59">
+        <v>0</v>
+      </c>
+      <c r="AH182" s="59">
+        <v>0</v>
+      </c>
+      <c r="AI182" s="59">
+        <v>0</v>
+      </c>
+      <c r="AJ182" s="59">
+        <v>0</v>
+      </c>
+      <c r="AK182" s="59">
+        <v>0</v>
+      </c>
+      <c r="AL182" s="59">
+        <v>0</v>
+      </c>
+      <c r="AM182" s="59">
+        <v>0</v>
+      </c>
+      <c r="AN182" s="59">
+        <v>0</v>
+      </c>
+      <c r="AO182" s="59">
+        <v>0</v>
+      </c>
       <c r="AP182" s="58">
         <f>Q182*AC182/1000000000</f>
         <v>0</v>
@@ -40032,31 +40182,81 @@
       <c r="N183" s="58"/>
       <c r="O183" s="58"/>
       <c r="P183" s="58"/>
-      <c r="Q183" s="58"/>
-      <c r="R183" s="58"/>
-      <c r="S183" s="58"/>
-      <c r="T183" s="58"/>
-      <c r="U183" s="58"/>
-      <c r="V183" s="58"/>
-      <c r="W183" s="58"/>
-      <c r="X183" s="58"/>
-      <c r="Y183" s="58"/>
-      <c r="Z183" s="58"/>
-      <c r="AA183" s="58"/>
-      <c r="AB183" s="58"/>
-      <c r="AC183" s="52"/>
-      <c r="AD183" s="59"/>
-      <c r="AE183" s="59"/>
-      <c r="AF183" s="59"/>
-      <c r="AG183" s="59"/>
-      <c r="AH183" s="59"/>
-      <c r="AI183" s="59"/>
-      <c r="AJ183" s="59"/>
-      <c r="AK183" s="59"/>
-      <c r="AL183" s="59"/>
-      <c r="AM183" s="59"/>
-      <c r="AN183" s="59"/>
-      <c r="AO183" s="59"/>
+      <c r="Q183" s="58">
+        <v>21.3</v>
+      </c>
+      <c r="R183" s="58">
+        <v>25.5</v>
+      </c>
+      <c r="S183" s="58">
+        <v>30.6</v>
+      </c>
+      <c r="T183" s="58">
+        <v>38.9</v>
+      </c>
+      <c r="U183" s="58">
+        <v>0</v>
+      </c>
+      <c r="V183" s="58">
+        <v>0</v>
+      </c>
+      <c r="W183" s="58">
+        <v>62.3</v>
+      </c>
+      <c r="X183" s="58">
+        <v>76.2</v>
+      </c>
+      <c r="Y183" s="58">
+        <v>0</v>
+      </c>
+      <c r="Z183" s="58">
+        <v>0</v>
+      </c>
+      <c r="AA183" s="58">
+        <v>0</v>
+      </c>
+      <c r="AB183" s="58">
+        <v>0</v>
+      </c>
+      <c r="AC183" s="52">
+        <v>0</v>
+      </c>
+      <c r="AD183" s="59">
+        <v>0</v>
+      </c>
+      <c r="AE183" s="59">
+        <v>0</v>
+      </c>
+      <c r="AF183" s="59">
+        <v>0</v>
+      </c>
+      <c r="AG183" s="59">
+        <v>0</v>
+      </c>
+      <c r="AH183" s="59">
+        <v>0</v>
+      </c>
+      <c r="AI183" s="59">
+        <v>0</v>
+      </c>
+      <c r="AJ183" s="59">
+        <v>0</v>
+      </c>
+      <c r="AK183" s="59">
+        <v>0</v>
+      </c>
+      <c r="AL183" s="59">
+        <v>0</v>
+      </c>
+      <c r="AM183" s="59">
+        <v>0</v>
+      </c>
+      <c r="AN183" s="59">
+        <v>0</v>
+      </c>
+      <c r="AO183" s="59">
+        <v>0</v>
+      </c>
       <c r="AP183" s="58">
         <f>Q183*AC183/1000000000</f>
         <v>0</v>
@@ -40216,31 +40416,81 @@
       <c r="N184" s="58"/>
       <c r="O184" s="58"/>
       <c r="P184" s="58"/>
-      <c r="Q184" s="58"/>
-      <c r="R184" s="58"/>
-      <c r="S184" s="58"/>
-      <c r="T184" s="58"/>
-      <c r="U184" s="58"/>
-      <c r="V184" s="58"/>
-      <c r="W184" s="58"/>
-      <c r="X184" s="58"/>
-      <c r="Y184" s="58"/>
-      <c r="Z184" s="58"/>
-      <c r="AA184" s="58"/>
-      <c r="AB184" s="58"/>
-      <c r="AC184" s="52"/>
-      <c r="AD184" s="59"/>
-      <c r="AE184" s="59"/>
-      <c r="AF184" s="59"/>
-      <c r="AG184" s="59"/>
-      <c r="AH184" s="59"/>
-      <c r="AI184" s="59"/>
-      <c r="AJ184" s="59"/>
-      <c r="AK184" s="59"/>
-      <c r="AL184" s="59"/>
-      <c r="AM184" s="59"/>
-      <c r="AN184" s="59"/>
-      <c r="AO184" s="59"/>
+      <c r="Q184" s="58">
+        <v>1.8</v>
+      </c>
+      <c r="R184" s="58">
+        <v>1.9</v>
+      </c>
+      <c r="S184" s="58">
+        <v>2</v>
+      </c>
+      <c r="T184" s="58">
+        <v>2.2</v>
+      </c>
+      <c r="U184" s="58">
+        <v>0</v>
+      </c>
+      <c r="V184" s="58">
+        <v>0</v>
+      </c>
+      <c r="W184" s="58">
+        <v>2.6</v>
+      </c>
+      <c r="X184" s="58">
+        <v>2.8</v>
+      </c>
+      <c r="Y184" s="58">
+        <v>0</v>
+      </c>
+      <c r="Z184" s="58">
+        <v>0</v>
+      </c>
+      <c r="AA184" s="58">
+        <v>0</v>
+      </c>
+      <c r="AB184" s="58">
+        <v>0</v>
+      </c>
+      <c r="AC184" s="52">
+        <v>0</v>
+      </c>
+      <c r="AD184" s="59">
+        <v>0</v>
+      </c>
+      <c r="AE184" s="59">
+        <v>0</v>
+      </c>
+      <c r="AF184" s="59">
+        <v>0</v>
+      </c>
+      <c r="AG184" s="59">
+        <v>0</v>
+      </c>
+      <c r="AH184" s="59">
+        <v>0</v>
+      </c>
+      <c r="AI184" s="59">
+        <v>0</v>
+      </c>
+      <c r="AJ184" s="59">
+        <v>0</v>
+      </c>
+      <c r="AK184" s="59">
+        <v>0</v>
+      </c>
+      <c r="AL184" s="59">
+        <v>0</v>
+      </c>
+      <c r="AM184" s="59">
+        <v>0</v>
+      </c>
+      <c r="AN184" s="59">
+        <v>0</v>
+      </c>
+      <c r="AO184" s="59">
+        <v>0</v>
+      </c>
       <c r="AP184" s="58">
         <f>Q184*AC184/1000000000</f>
         <v>0</v>
@@ -40400,31 +40650,81 @@
       <c r="N185" s="58"/>
       <c r="O185" s="58"/>
       <c r="P185" s="58"/>
-      <c r="Q185" s="58"/>
-      <c r="R185" s="58"/>
-      <c r="S185" s="58"/>
-      <c r="T185" s="58"/>
-      <c r="U185" s="58"/>
-      <c r="V185" s="58"/>
-      <c r="W185" s="58"/>
-      <c r="X185" s="58"/>
-      <c r="Y185" s="58"/>
-      <c r="Z185" s="58"/>
-      <c r="AA185" s="58"/>
-      <c r="AB185" s="58"/>
-      <c r="AC185" s="52"/>
-      <c r="AD185" s="59"/>
-      <c r="AE185" s="59"/>
-      <c r="AF185" s="59"/>
-      <c r="AG185" s="59"/>
-      <c r="AH185" s="59"/>
-      <c r="AI185" s="59"/>
-      <c r="AJ185" s="59"/>
-      <c r="AK185" s="59"/>
-      <c r="AL185" s="59"/>
-      <c r="AM185" s="59"/>
-      <c r="AN185" s="59"/>
-      <c r="AO185" s="59"/>
+      <c r="Q185" s="58">
+        <v>52.8</v>
+      </c>
+      <c r="R185" s="58">
+        <v>70.4</v>
+      </c>
+      <c r="S185" s="58">
+        <v>76</v>
+      </c>
+      <c r="T185" s="58">
+        <v>82.8</v>
+      </c>
+      <c r="U185" s="58">
+        <v>0</v>
+      </c>
+      <c r="V185" s="58">
+        <v>0</v>
+      </c>
+      <c r="W185" s="58">
+        <v>102.3</v>
+      </c>
+      <c r="X185" s="58">
+        <v>115.4</v>
+      </c>
+      <c r="Y185" s="58">
+        <v>0</v>
+      </c>
+      <c r="Z185" s="58">
+        <v>0</v>
+      </c>
+      <c r="AA185" s="58">
+        <v>0</v>
+      </c>
+      <c r="AB185" s="58">
+        <v>0</v>
+      </c>
+      <c r="AC185" s="52">
+        <v>0</v>
+      </c>
+      <c r="AD185" s="59">
+        <v>0</v>
+      </c>
+      <c r="AE185" s="59">
+        <v>0</v>
+      </c>
+      <c r="AF185" s="59">
+        <v>0</v>
+      </c>
+      <c r="AG185" s="59">
+        <v>0</v>
+      </c>
+      <c r="AH185" s="59">
+        <v>0</v>
+      </c>
+      <c r="AI185" s="59">
+        <v>0</v>
+      </c>
+      <c r="AJ185" s="59">
+        <v>0</v>
+      </c>
+      <c r="AK185" s="59">
+        <v>0</v>
+      </c>
+      <c r="AL185" s="59">
+        <v>0</v>
+      </c>
+      <c r="AM185" s="59">
+        <v>0</v>
+      </c>
+      <c r="AN185" s="59">
+        <v>0</v>
+      </c>
+      <c r="AO185" s="59">
+        <v>0</v>
+      </c>
       <c r="AP185" s="58">
         <f>Q185*AC185/1000000000</f>
         <v>0</v>
@@ -40584,31 +40884,81 @@
       <c r="N186" s="58"/>
       <c r="O186" s="58"/>
       <c r="P186" s="58"/>
-      <c r="Q186" s="58"/>
-      <c r="R186" s="58"/>
-      <c r="S186" s="58"/>
-      <c r="T186" s="58"/>
-      <c r="U186" s="58"/>
-      <c r="V186" s="58"/>
-      <c r="W186" s="58"/>
-      <c r="X186" s="58"/>
-      <c r="Y186" s="58"/>
-      <c r="Z186" s="58"/>
-      <c r="AA186" s="58"/>
-      <c r="AB186" s="58"/>
-      <c r="AC186" s="52"/>
-      <c r="AD186" s="59"/>
-      <c r="AE186" s="59"/>
-      <c r="AF186" s="59"/>
-      <c r="AG186" s="59"/>
-      <c r="AH186" s="59"/>
-      <c r="AI186" s="59"/>
-      <c r="AJ186" s="59"/>
-      <c r="AK186" s="59"/>
-      <c r="AL186" s="59"/>
-      <c r="AM186" s="59"/>
-      <c r="AN186" s="59"/>
-      <c r="AO186" s="59"/>
+      <c r="Q186" s="58">
+        <v>9.9</v>
+      </c>
+      <c r="R186" s="58">
+        <v>2.3</v>
+      </c>
+      <c r="S186" s="58">
+        <v>2.5</v>
+      </c>
+      <c r="T186" s="58">
+        <v>2.7</v>
+      </c>
+      <c r="U186" s="58">
+        <v>0</v>
+      </c>
+      <c r="V186" s="58">
+        <v>0</v>
+      </c>
+      <c r="W186" s="58">
+        <v>3.5</v>
+      </c>
+      <c r="X186" s="58">
+        <v>3.9</v>
+      </c>
+      <c r="Y186" s="58">
+        <v>0</v>
+      </c>
+      <c r="Z186" s="58">
+        <v>0</v>
+      </c>
+      <c r="AA186" s="58">
+        <v>0</v>
+      </c>
+      <c r="AB186" s="58">
+        <v>0</v>
+      </c>
+      <c r="AC186" s="52">
+        <v>0</v>
+      </c>
+      <c r="AD186" s="59">
+        <v>0</v>
+      </c>
+      <c r="AE186" s="59">
+        <v>0</v>
+      </c>
+      <c r="AF186" s="59">
+        <v>0</v>
+      </c>
+      <c r="AG186" s="59">
+        <v>0</v>
+      </c>
+      <c r="AH186" s="59">
+        <v>0</v>
+      </c>
+      <c r="AI186" s="59">
+        <v>0</v>
+      </c>
+      <c r="AJ186" s="59">
+        <v>0</v>
+      </c>
+      <c r="AK186" s="59">
+        <v>0</v>
+      </c>
+      <c r="AL186" s="59">
+        <v>0</v>
+      </c>
+      <c r="AM186" s="59">
+        <v>0</v>
+      </c>
+      <c r="AN186" s="59">
+        <v>0</v>
+      </c>
+      <c r="AO186" s="59">
+        <v>0</v>
+      </c>
       <c r="AP186" s="58">
         <f>Q186*AC186/1000000000</f>
         <v>0</v>
@@ -40768,31 +41118,81 @@
       <c r="N187" s="58"/>
       <c r="O187" s="58"/>
       <c r="P187" s="58"/>
-      <c r="Q187" s="58"/>
-      <c r="R187" s="58"/>
-      <c r="S187" s="58"/>
-      <c r="T187" s="58"/>
-      <c r="U187" s="58"/>
-      <c r="V187" s="58"/>
-      <c r="W187" s="58"/>
-      <c r="X187" s="58"/>
-      <c r="Y187" s="58"/>
-      <c r="Z187" s="58"/>
-      <c r="AA187" s="58"/>
-      <c r="AB187" s="58"/>
-      <c r="AC187" s="52"/>
-      <c r="AD187" s="59"/>
-      <c r="AE187" s="59"/>
-      <c r="AF187" s="59"/>
-      <c r="AG187" s="59"/>
-      <c r="AH187" s="59"/>
-      <c r="AI187" s="59"/>
-      <c r="AJ187" s="59"/>
-      <c r="AK187" s="59"/>
-      <c r="AL187" s="59"/>
-      <c r="AM187" s="59"/>
-      <c r="AN187" s="59"/>
-      <c r="AO187" s="59"/>
+      <c r="Q187" s="58">
+        <v>8.7</v>
+      </c>
+      <c r="R187" s="58">
+        <v>9.4</v>
+      </c>
+      <c r="S187" s="58">
+        <v>10.1</v>
+      </c>
+      <c r="T187" s="58">
+        <v>11.4</v>
+      </c>
+      <c r="U187" s="58">
+        <v>0</v>
+      </c>
+      <c r="V187" s="58">
+        <v>0</v>
+      </c>
+      <c r="W187" s="58">
+        <v>14.4</v>
+      </c>
+      <c r="X187" s="58">
+        <v>15.8</v>
+      </c>
+      <c r="Y187" s="58">
+        <v>0</v>
+      </c>
+      <c r="Z187" s="58">
+        <v>0</v>
+      </c>
+      <c r="AA187" s="58">
+        <v>0</v>
+      </c>
+      <c r="AB187" s="58">
+        <v>0</v>
+      </c>
+      <c r="AC187" s="52">
+        <v>0</v>
+      </c>
+      <c r="AD187" s="59">
+        <v>0</v>
+      </c>
+      <c r="AE187" s="59">
+        <v>0</v>
+      </c>
+      <c r="AF187" s="59">
+        <v>0</v>
+      </c>
+      <c r="AG187" s="59">
+        <v>0</v>
+      </c>
+      <c r="AH187" s="59">
+        <v>0</v>
+      </c>
+      <c r="AI187" s="59">
+        <v>0</v>
+      </c>
+      <c r="AJ187" s="59">
+        <v>0</v>
+      </c>
+      <c r="AK187" s="59">
+        <v>0</v>
+      </c>
+      <c r="AL187" s="59">
+        <v>0</v>
+      </c>
+      <c r="AM187" s="59">
+        <v>0</v>
+      </c>
+      <c r="AN187" s="59">
+        <v>0</v>
+      </c>
+      <c r="AO187" s="59">
+        <v>0</v>
+      </c>
       <c r="AP187" s="58">
         <f>Q187*AC187/1000000000</f>
         <v>0</v>
@@ -40952,31 +41352,81 @@
       <c r="N188" s="58"/>
       <c r="O188" s="58"/>
       <c r="P188" s="58"/>
-      <c r="Q188" s="58"/>
-      <c r="R188" s="58"/>
-      <c r="S188" s="58"/>
-      <c r="T188" s="58"/>
-      <c r="U188" s="58"/>
-      <c r="V188" s="58"/>
-      <c r="W188" s="58"/>
-      <c r="X188" s="58"/>
-      <c r="Y188" s="58"/>
-      <c r="Z188" s="58"/>
-      <c r="AA188" s="58"/>
-      <c r="AB188" s="58"/>
-      <c r="AC188" s="52"/>
-      <c r="AD188" s="59"/>
-      <c r="AE188" s="59"/>
-      <c r="AF188" s="59"/>
-      <c r="AG188" s="59"/>
-      <c r="AH188" s="59"/>
-      <c r="AI188" s="59"/>
-      <c r="AJ188" s="59"/>
-      <c r="AK188" s="59"/>
-      <c r="AL188" s="59"/>
-      <c r="AM188" s="59"/>
-      <c r="AN188" s="59"/>
-      <c r="AO188" s="59"/>
+      <c r="Q188" s="58">
+        <v>55.2</v>
+      </c>
+      <c r="R188" s="58">
+        <v>49.8</v>
+      </c>
+      <c r="S188" s="58">
+        <v>53.3</v>
+      </c>
+      <c r="T188" s="58">
+        <v>57.9</v>
+      </c>
+      <c r="U188" s="58">
+        <v>0</v>
+      </c>
+      <c r="V188" s="58">
+        <v>0</v>
+      </c>
+      <c r="W188" s="58">
+        <v>65.2</v>
+      </c>
+      <c r="X188" s="58">
+        <v>67</v>
+      </c>
+      <c r="Y188" s="58">
+        <v>0</v>
+      </c>
+      <c r="Z188" s="58">
+        <v>0</v>
+      </c>
+      <c r="AA188" s="58">
+        <v>0</v>
+      </c>
+      <c r="AB188" s="58">
+        <v>0</v>
+      </c>
+      <c r="AC188" s="52">
+        <v>0</v>
+      </c>
+      <c r="AD188" s="59">
+        <v>0</v>
+      </c>
+      <c r="AE188" s="59">
+        <v>0</v>
+      </c>
+      <c r="AF188" s="59">
+        <v>0</v>
+      </c>
+      <c r="AG188" s="59">
+        <v>0</v>
+      </c>
+      <c r="AH188" s="59">
+        <v>0</v>
+      </c>
+      <c r="AI188" s="59">
+        <v>0</v>
+      </c>
+      <c r="AJ188" s="59">
+        <v>0</v>
+      </c>
+      <c r="AK188" s="59">
+        <v>0</v>
+      </c>
+      <c r="AL188" s="59">
+        <v>0</v>
+      </c>
+      <c r="AM188" s="59">
+        <v>0</v>
+      </c>
+      <c r="AN188" s="59">
+        <v>0</v>
+      </c>
+      <c r="AO188" s="59">
+        <v>0</v>
+      </c>
       <c r="AP188" s="58">
         <f>Q188*AC188/1000000000</f>
         <v>0</v>
@@ -41136,31 +41586,81 @@
       <c r="N189" s="58"/>
       <c r="O189" s="58"/>
       <c r="P189" s="58"/>
-      <c r="Q189" s="58"/>
-      <c r="R189" s="58"/>
-      <c r="S189" s="58"/>
-      <c r="T189" s="58"/>
-      <c r="U189" s="58"/>
-      <c r="V189" s="58"/>
-      <c r="W189" s="58"/>
-      <c r="X189" s="58"/>
-      <c r="Y189" s="58"/>
-      <c r="Z189" s="58"/>
-      <c r="AA189" s="58"/>
-      <c r="AB189" s="58"/>
-      <c r="AC189" s="52"/>
-      <c r="AD189" s="59"/>
-      <c r="AE189" s="59"/>
-      <c r="AF189" s="59"/>
-      <c r="AG189" s="59"/>
-      <c r="AH189" s="59"/>
-      <c r="AI189" s="59"/>
-      <c r="AJ189" s="59"/>
-      <c r="AK189" s="59"/>
-      <c r="AL189" s="59"/>
-      <c r="AM189" s="59"/>
-      <c r="AN189" s="59"/>
-      <c r="AO189" s="59"/>
+      <c r="Q189" s="58">
+        <v>1.7</v>
+      </c>
+      <c r="R189" s="58">
+        <v>1.9</v>
+      </c>
+      <c r="S189" s="58">
+        <v>2</v>
+      </c>
+      <c r="T189" s="58">
+        <v>2.2</v>
+      </c>
+      <c r="U189" s="58">
+        <v>0</v>
+      </c>
+      <c r="V189" s="58">
+        <v>0</v>
+      </c>
+      <c r="W189" s="58">
+        <v>2.5</v>
+      </c>
+      <c r="X189" s="58">
+        <v>2.7</v>
+      </c>
+      <c r="Y189" s="58">
+        <v>0</v>
+      </c>
+      <c r="Z189" s="58">
+        <v>0</v>
+      </c>
+      <c r="AA189" s="58">
+        <v>0</v>
+      </c>
+      <c r="AB189" s="58">
+        <v>0</v>
+      </c>
+      <c r="AC189" s="52">
+        <v>0</v>
+      </c>
+      <c r="AD189" s="59">
+        <v>0</v>
+      </c>
+      <c r="AE189" s="59">
+        <v>0</v>
+      </c>
+      <c r="AF189" s="59">
+        <v>0</v>
+      </c>
+      <c r="AG189" s="59">
+        <v>0</v>
+      </c>
+      <c r="AH189" s="59">
+        <v>0</v>
+      </c>
+      <c r="AI189" s="59">
+        <v>0</v>
+      </c>
+      <c r="AJ189" s="59">
+        <v>0</v>
+      </c>
+      <c r="AK189" s="59">
+        <v>0</v>
+      </c>
+      <c r="AL189" s="59">
+        <v>0</v>
+      </c>
+      <c r="AM189" s="59">
+        <v>0</v>
+      </c>
+      <c r="AN189" s="59">
+        <v>0</v>
+      </c>
+      <c r="AO189" s="59">
+        <v>0</v>
+      </c>
       <c r="AP189" s="58">
         <f>Q189*AC189/1000000000</f>
         <v>0</v>
@@ -41320,31 +41820,81 @@
       <c r="N190" s="58"/>
       <c r="O190" s="58"/>
       <c r="P190" s="58"/>
-      <c r="Q190" s="58"/>
-      <c r="R190" s="58"/>
-      <c r="S190" s="58"/>
-      <c r="T190" s="58"/>
-      <c r="U190" s="58"/>
-      <c r="V190" s="58"/>
-      <c r="W190" s="58"/>
-      <c r="X190" s="58"/>
-      <c r="Y190" s="58"/>
-      <c r="Z190" s="58"/>
-      <c r="AA190" s="58"/>
-      <c r="AB190" s="58"/>
-      <c r="AC190" s="52"/>
-      <c r="AD190" s="59"/>
-      <c r="AE190" s="59"/>
-      <c r="AF190" s="59"/>
-      <c r="AG190" s="59"/>
-      <c r="AH190" s="59"/>
-      <c r="AI190" s="59"/>
-      <c r="AJ190" s="59"/>
-      <c r="AK190" s="59"/>
-      <c r="AL190" s="59"/>
-      <c r="AM190" s="59"/>
-      <c r="AN190" s="59"/>
-      <c r="AO190" s="59"/>
+      <c r="Q190" s="58">
+        <v>2.4</v>
+      </c>
+      <c r="R190" s="58">
+        <v>2.3</v>
+      </c>
+      <c r="S190" s="58">
+        <v>3.2</v>
+      </c>
+      <c r="T190" s="58">
+        <v>0.4</v>
+      </c>
+      <c r="U190" s="58">
+        <v>0</v>
+      </c>
+      <c r="V190" s="58">
+        <v>0</v>
+      </c>
+      <c r="W190" s="58">
+        <v>0.5</v>
+      </c>
+      <c r="X190" s="58">
+        <v>4.1</v>
+      </c>
+      <c r="Y190" s="58">
+        <v>0</v>
+      </c>
+      <c r="Z190" s="58">
+        <v>0</v>
+      </c>
+      <c r="AA190" s="58">
+        <v>0</v>
+      </c>
+      <c r="AB190" s="58">
+        <v>0</v>
+      </c>
+      <c r="AC190" s="52">
+        <v>0</v>
+      </c>
+      <c r="AD190" s="59">
+        <v>0</v>
+      </c>
+      <c r="AE190" s="59">
+        <v>0</v>
+      </c>
+      <c r="AF190" s="59">
+        <v>0</v>
+      </c>
+      <c r="AG190" s="59">
+        <v>0</v>
+      </c>
+      <c r="AH190" s="59">
+        <v>0</v>
+      </c>
+      <c r="AI190" s="59">
+        <v>0</v>
+      </c>
+      <c r="AJ190" s="59">
+        <v>0</v>
+      </c>
+      <c r="AK190" s="59">
+        <v>0</v>
+      </c>
+      <c r="AL190" s="59">
+        <v>0</v>
+      </c>
+      <c r="AM190" s="59">
+        <v>0</v>
+      </c>
+      <c r="AN190" s="59">
+        <v>0</v>
+      </c>
+      <c r="AO190" s="59">
+        <v>0</v>
+      </c>
       <c r="AP190" s="58">
         <f>Q190*AC190/1000000000</f>
         <v>0</v>
@@ -41504,31 +42054,81 @@
       <c r="N191" s="58"/>
       <c r="O191" s="58"/>
       <c r="P191" s="58"/>
-      <c r="Q191" s="58"/>
-      <c r="R191" s="58"/>
-      <c r="S191" s="58"/>
-      <c r="T191" s="58"/>
-      <c r="U191" s="58"/>
-      <c r="V191" s="58"/>
-      <c r="W191" s="58"/>
-      <c r="X191" s="58"/>
-      <c r="Y191" s="58"/>
-      <c r="Z191" s="58"/>
-      <c r="AA191" s="58"/>
-      <c r="AB191" s="58"/>
-      <c r="AC191" s="52"/>
-      <c r="AD191" s="59"/>
-      <c r="AE191" s="59"/>
-      <c r="AF191" s="59"/>
-      <c r="AG191" s="59"/>
-      <c r="AH191" s="59"/>
-      <c r="AI191" s="59"/>
-      <c r="AJ191" s="59"/>
-      <c r="AK191" s="59"/>
-      <c r="AL191" s="59"/>
-      <c r="AM191" s="59"/>
-      <c r="AN191" s="59"/>
-      <c r="AO191" s="59"/>
+      <c r="Q191" s="58">
+        <v>15.2</v>
+      </c>
+      <c r="R191" s="58">
+        <v>16.6</v>
+      </c>
+      <c r="S191" s="58">
+        <v>18.1</v>
+      </c>
+      <c r="T191" s="58">
+        <v>19.2</v>
+      </c>
+      <c r="U191" s="58">
+        <v>0</v>
+      </c>
+      <c r="V191" s="58">
+        <v>0</v>
+      </c>
+      <c r="W191" s="58">
+        <v>22.9</v>
+      </c>
+      <c r="X191" s="58">
+        <v>25.4</v>
+      </c>
+      <c r="Y191" s="58">
+        <v>0</v>
+      </c>
+      <c r="Z191" s="58">
+        <v>0</v>
+      </c>
+      <c r="AA191" s="58">
+        <v>0</v>
+      </c>
+      <c r="AB191" s="58">
+        <v>0</v>
+      </c>
+      <c r="AC191" s="52">
+        <v>0</v>
+      </c>
+      <c r="AD191" s="59">
+        <v>0</v>
+      </c>
+      <c r="AE191" s="59">
+        <v>0</v>
+      </c>
+      <c r="AF191" s="59">
+        <v>0</v>
+      </c>
+      <c r="AG191" s="59">
+        <v>0</v>
+      </c>
+      <c r="AH191" s="59">
+        <v>0</v>
+      </c>
+      <c r="AI191" s="59">
+        <v>0</v>
+      </c>
+      <c r="AJ191" s="59">
+        <v>0</v>
+      </c>
+      <c r="AK191" s="59">
+        <v>0</v>
+      </c>
+      <c r="AL191" s="59">
+        <v>0</v>
+      </c>
+      <c r="AM191" s="59">
+        <v>0</v>
+      </c>
+      <c r="AN191" s="59">
+        <v>0</v>
+      </c>
+      <c r="AO191" s="59">
+        <v>0</v>
+      </c>
       <c r="AP191" s="58">
         <f>Q191*AC191/1000000000</f>
         <v>0</v>
@@ -41688,31 +42288,81 @@
       <c r="N192" s="58"/>
       <c r="O192" s="58"/>
       <c r="P192" s="58"/>
-      <c r="Q192" s="58"/>
-      <c r="R192" s="58"/>
-      <c r="S192" s="58"/>
-      <c r="T192" s="58"/>
-      <c r="U192" s="58"/>
-      <c r="V192" s="58"/>
-      <c r="W192" s="58"/>
-      <c r="X192" s="58"/>
-      <c r="Y192" s="58"/>
-      <c r="Z192" s="58"/>
-      <c r="AA192" s="58"/>
-      <c r="AB192" s="58"/>
-      <c r="AC192" s="52"/>
-      <c r="AD192" s="59"/>
-      <c r="AE192" s="59"/>
-      <c r="AF192" s="59"/>
-      <c r="AG192" s="59"/>
-      <c r="AH192" s="59"/>
-      <c r="AI192" s="59"/>
-      <c r="AJ192" s="59"/>
-      <c r="AK192" s="59"/>
-      <c r="AL192" s="59"/>
-      <c r="AM192" s="59"/>
-      <c r="AN192" s="59"/>
-      <c r="AO192" s="59"/>
+      <c r="Q192" s="58">
+        <v>6.3</v>
+      </c>
+      <c r="R192" s="58">
+        <v>6.6</v>
+      </c>
+      <c r="S192" s="58">
+        <v>7.1</v>
+      </c>
+      <c r="T192" s="58">
+        <v>7.6</v>
+      </c>
+      <c r="U192" s="58">
+        <v>0</v>
+      </c>
+      <c r="V192" s="58">
+        <v>0</v>
+      </c>
+      <c r="W192" s="58">
+        <v>8.8</v>
+      </c>
+      <c r="X192" s="58">
+        <v>9.4</v>
+      </c>
+      <c r="Y192" s="58">
+        <v>0</v>
+      </c>
+      <c r="Z192" s="58">
+        <v>0</v>
+      </c>
+      <c r="AA192" s="58">
+        <v>0</v>
+      </c>
+      <c r="AB192" s="58">
+        <v>0</v>
+      </c>
+      <c r="AC192" s="52">
+        <v>0</v>
+      </c>
+      <c r="AD192" s="59">
+        <v>0</v>
+      </c>
+      <c r="AE192" s="59">
+        <v>0</v>
+      </c>
+      <c r="AF192" s="59">
+        <v>0</v>
+      </c>
+      <c r="AG192" s="59">
+        <v>0</v>
+      </c>
+      <c r="AH192" s="59">
+        <v>0</v>
+      </c>
+      <c r="AI192" s="59">
+        <v>0</v>
+      </c>
+      <c r="AJ192" s="59">
+        <v>0</v>
+      </c>
+      <c r="AK192" s="59">
+        <v>0</v>
+      </c>
+      <c r="AL192" s="59">
+        <v>0</v>
+      </c>
+      <c r="AM192" s="59">
+        <v>0</v>
+      </c>
+      <c r="AN192" s="59">
+        <v>0</v>
+      </c>
+      <c r="AO192" s="59">
+        <v>0</v>
+      </c>
       <c r="AP192" s="58">
         <f>Q192*AC192/1000000000</f>
         <v>0</v>
@@ -41872,31 +42522,81 @@
       <c r="N193" s="58"/>
       <c r="O193" s="58"/>
       <c r="P193" s="58"/>
-      <c r="Q193" s="58"/>
-      <c r="R193" s="58"/>
-      <c r="S193" s="58"/>
-      <c r="T193" s="58"/>
-      <c r="U193" s="58"/>
-      <c r="V193" s="58"/>
-      <c r="W193" s="58"/>
-      <c r="X193" s="58"/>
-      <c r="Y193" s="58"/>
-      <c r="Z193" s="58"/>
-      <c r="AA193" s="58"/>
-      <c r="AB193" s="58"/>
-      <c r="AC193" s="52"/>
-      <c r="AD193" s="59"/>
-      <c r="AE193" s="59"/>
-      <c r="AF193" s="59"/>
-      <c r="AG193" s="59"/>
-      <c r="AH193" s="59"/>
-      <c r="AI193" s="59"/>
-      <c r="AJ193" s="59"/>
-      <c r="AK193" s="59"/>
-      <c r="AL193" s="59"/>
-      <c r="AM193" s="59"/>
-      <c r="AN193" s="59"/>
-      <c r="AO193" s="59"/>
+      <c r="Q193" s="58">
+        <v>211.6</v>
+      </c>
+      <c r="R193" s="58">
+        <v>233.3</v>
+      </c>
+      <c r="S193" s="58">
+        <v>244.5</v>
+      </c>
+      <c r="T193" s="58">
+        <v>290.4</v>
+      </c>
+      <c r="U193" s="58">
+        <v>0</v>
+      </c>
+      <c r="V193" s="58">
+        <v>0</v>
+      </c>
+      <c r="W193" s="58">
+        <v>343.6</v>
+      </c>
+      <c r="X193" s="58">
+        <v>374.9</v>
+      </c>
+      <c r="Y193" s="58">
+        <v>0</v>
+      </c>
+      <c r="Z193" s="58">
+        <v>0</v>
+      </c>
+      <c r="AA193" s="58">
+        <v>0</v>
+      </c>
+      <c r="AB193" s="58">
+        <v>0</v>
+      </c>
+      <c r="AC193" s="52">
+        <v>0</v>
+      </c>
+      <c r="AD193" s="59">
+        <v>0</v>
+      </c>
+      <c r="AE193" s="59">
+        <v>0</v>
+      </c>
+      <c r="AF193" s="59">
+        <v>0</v>
+      </c>
+      <c r="AG193" s="59">
+        <v>0</v>
+      </c>
+      <c r="AH193" s="59">
+        <v>0</v>
+      </c>
+      <c r="AI193" s="59">
+        <v>0</v>
+      </c>
+      <c r="AJ193" s="59">
+        <v>0</v>
+      </c>
+      <c r="AK193" s="59">
+        <v>0</v>
+      </c>
+      <c r="AL193" s="59">
+        <v>0</v>
+      </c>
+      <c r="AM193" s="59">
+        <v>0</v>
+      </c>
+      <c r="AN193" s="59">
+        <v>0</v>
+      </c>
+      <c r="AO193" s="59">
+        <v>0</v>
+      </c>
       <c r="AP193" s="58">
         <f>Q193*AC193/1000000000</f>
         <v>0</v>
@@ -42056,31 +42756,81 @@
       <c r="N194" s="58"/>
       <c r="O194" s="58"/>
       <c r="P194" s="58"/>
-      <c r="Q194" s="58"/>
-      <c r="R194" s="58"/>
-      <c r="S194" s="58"/>
-      <c r="T194" s="58"/>
-      <c r="U194" s="58"/>
-      <c r="V194" s="58"/>
-      <c r="W194" s="58"/>
-      <c r="X194" s="58"/>
-      <c r="Y194" s="58"/>
-      <c r="Z194" s="58"/>
-      <c r="AA194" s="58"/>
-      <c r="AB194" s="58"/>
-      <c r="AC194" s="52"/>
-      <c r="AD194" s="59"/>
-      <c r="AE194" s="59"/>
-      <c r="AF194" s="59"/>
-      <c r="AG194" s="59"/>
-      <c r="AH194" s="59"/>
-      <c r="AI194" s="59"/>
-      <c r="AJ194" s="59"/>
-      <c r="AK194" s="59"/>
-      <c r="AL194" s="59"/>
-      <c r="AM194" s="59"/>
-      <c r="AN194" s="59"/>
-      <c r="AO194" s="59"/>
+      <c r="Q194" s="58">
+        <v>179.9</v>
+      </c>
+      <c r="R194" s="58">
+        <v>192.8</v>
+      </c>
+      <c r="S194" s="58">
+        <v>203.9</v>
+      </c>
+      <c r="T194" s="58">
+        <v>172.7</v>
+      </c>
+      <c r="U194" s="58">
+        <v>0</v>
+      </c>
+      <c r="V194" s="58">
+        <v>0</v>
+      </c>
+      <c r="W194" s="58">
+        <v>248.7</v>
+      </c>
+      <c r="X194" s="58">
+        <v>310.6</v>
+      </c>
+      <c r="Y194" s="58">
+        <v>0</v>
+      </c>
+      <c r="Z194" s="58">
+        <v>0</v>
+      </c>
+      <c r="AA194" s="58">
+        <v>0</v>
+      </c>
+      <c r="AB194" s="58">
+        <v>0</v>
+      </c>
+      <c r="AC194" s="52">
+        <v>0</v>
+      </c>
+      <c r="AD194" s="59">
+        <v>0</v>
+      </c>
+      <c r="AE194" s="59">
+        <v>0</v>
+      </c>
+      <c r="AF194" s="59">
+        <v>0</v>
+      </c>
+      <c r="AG194" s="59">
+        <v>0</v>
+      </c>
+      <c r="AH194" s="59">
+        <v>0</v>
+      </c>
+      <c r="AI194" s="59">
+        <v>0</v>
+      </c>
+      <c r="AJ194" s="59">
+        <v>0</v>
+      </c>
+      <c r="AK194" s="59">
+        <v>0</v>
+      </c>
+      <c r="AL194" s="59">
+        <v>0</v>
+      </c>
+      <c r="AM194" s="59">
+        <v>0</v>
+      </c>
+      <c r="AN194" s="59">
+        <v>0</v>
+      </c>
+      <c r="AO194" s="59">
+        <v>0</v>
+      </c>
       <c r="AP194" s="58">
         <f>Q194*AC194/1000000000</f>
         <v>0</v>
@@ -42263,66 +43013,80 @@
         <v>0</v>
       </c>
       <c r="Q195" s="52">
-        <f>SUM(Q196:Q210)</f>
-        <v>0</v>
+        <v>18.5</v>
       </c>
       <c r="R195" s="52">
-        <f>SUM(R196:R210)</f>
-        <v>0</v>
+        <v>17.9</v>
       </c>
       <c r="S195" s="52">
-        <f>SUM(S196:S210)</f>
-        <v>0</v>
+        <v>18.6</v>
       </c>
       <c r="T195" s="52">
-        <f>SUM(T196:T210)</f>
-        <v>0</v>
+        <v>24.3</v>
       </c>
       <c r="U195" s="52">
-        <f>SUM(U196:U210)</f>
         <v>0</v>
       </c>
       <c r="V195" s="52">
-        <f>SUM(V196:V210)</f>
         <v>0</v>
       </c>
       <c r="W195" s="52">
-        <f>SUM(W196:W210)</f>
-        <v>0</v>
+        <v>26.6</v>
       </c>
       <c r="X195" s="52">
-        <f>SUM(X196:X210)</f>
-        <v>0</v>
+        <v>27.7</v>
       </c>
       <c r="Y195" s="52">
-        <f>SUM(Y196:Y210)</f>
         <v>0</v>
       </c>
       <c r="Z195" s="52">
-        <f>SUM(Z196:Z210)</f>
         <v>0</v>
       </c>
       <c r="AA195" s="52">
-        <f>SUM(AA196:AA210)</f>
         <v>0</v>
       </c>
       <c r="AB195" s="52">
-        <f>SUM(AB196:AB210)</f>
-        <v>0</v>
-      </c>
-      <c r="AC195" s="52"/>
-      <c r="AD195" s="59"/>
-      <c r="AE195" s="59"/>
-      <c r="AF195" s="59"/>
-      <c r="AG195" s="59"/>
-      <c r="AH195" s="59"/>
-      <c r="AI195" s="59"/>
-      <c r="AJ195" s="59"/>
-      <c r="AK195" s="59"/>
-      <c r="AL195" s="59"/>
-      <c r="AM195" s="59"/>
-      <c r="AN195" s="59"/>
-      <c r="AO195" s="59"/>
+        <v>0</v>
+      </c>
+      <c r="AC195" s="52">
+        <v>0</v>
+      </c>
+      <c r="AD195" s="59">
+        <v>0</v>
+      </c>
+      <c r="AE195" s="59">
+        <v>0</v>
+      </c>
+      <c r="AF195" s="59">
+        <v>0</v>
+      </c>
+      <c r="AG195" s="59">
+        <v>0</v>
+      </c>
+      <c r="AH195" s="59">
+        <v>0</v>
+      </c>
+      <c r="AI195" s="59">
+        <v>0</v>
+      </c>
+      <c r="AJ195" s="59">
+        <v>0</v>
+      </c>
+      <c r="AK195" s="59">
+        <v>0</v>
+      </c>
+      <c r="AL195" s="59">
+        <v>0</v>
+      </c>
+      <c r="AM195" s="59">
+        <v>0</v>
+      </c>
+      <c r="AN195" s="59">
+        <v>0</v>
+      </c>
+      <c r="AO195" s="59">
+        <v>0</v>
+      </c>
       <c r="AP195" s="58">
         <f>Q195*AC195/1000000000</f>
         <v>0</v>
@@ -42482,31 +43246,81 @@
       <c r="N196" s="58"/>
       <c r="O196" s="58"/>
       <c r="P196" s="58"/>
-      <c r="Q196" s="58"/>
-      <c r="R196" s="58"/>
-      <c r="S196" s="58"/>
-      <c r="T196" s="58"/>
-      <c r="U196" s="58"/>
-      <c r="V196" s="58"/>
-      <c r="W196" s="58"/>
-      <c r="X196" s="58"/>
-      <c r="Y196" s="58"/>
-      <c r="Z196" s="58"/>
-      <c r="AA196" s="58"/>
-      <c r="AB196" s="58"/>
-      <c r="AC196" s="52"/>
-      <c r="AD196" s="59"/>
-      <c r="AE196" s="59"/>
-      <c r="AF196" s="59"/>
-      <c r="AG196" s="59"/>
-      <c r="AH196" s="59"/>
-      <c r="AI196" s="59"/>
-      <c r="AJ196" s="59"/>
-      <c r="AK196" s="59"/>
-      <c r="AL196" s="59"/>
-      <c r="AM196" s="59"/>
-      <c r="AN196" s="59"/>
-      <c r="AO196" s="59"/>
+      <c r="Q196" s="58">
+        <v>28.1</v>
+      </c>
+      <c r="R196" s="58">
+        <v>31.5</v>
+      </c>
+      <c r="S196" s="58">
+        <v>34</v>
+      </c>
+      <c r="T196" s="58">
+        <v>48.5</v>
+      </c>
+      <c r="U196" s="58">
+        <v>0</v>
+      </c>
+      <c r="V196" s="58">
+        <v>0</v>
+      </c>
+      <c r="W196" s="58">
+        <v>63.4</v>
+      </c>
+      <c r="X196" s="58">
+        <v>71.6</v>
+      </c>
+      <c r="Y196" s="58">
+        <v>0</v>
+      </c>
+      <c r="Z196" s="58">
+        <v>0</v>
+      </c>
+      <c r="AA196" s="58">
+        <v>0</v>
+      </c>
+      <c r="AB196" s="58">
+        <v>0</v>
+      </c>
+      <c r="AC196" s="52">
+        <v>0</v>
+      </c>
+      <c r="AD196" s="59">
+        <v>0</v>
+      </c>
+      <c r="AE196" s="59">
+        <v>0</v>
+      </c>
+      <c r="AF196" s="59">
+        <v>0</v>
+      </c>
+      <c r="AG196" s="59">
+        <v>0</v>
+      </c>
+      <c r="AH196" s="59">
+        <v>0</v>
+      </c>
+      <c r="AI196" s="59">
+        <v>0</v>
+      </c>
+      <c r="AJ196" s="59">
+        <v>0</v>
+      </c>
+      <c r="AK196" s="59">
+        <v>0</v>
+      </c>
+      <c r="AL196" s="59">
+        <v>0</v>
+      </c>
+      <c r="AM196" s="59">
+        <v>0</v>
+      </c>
+      <c r="AN196" s="59">
+        <v>0</v>
+      </c>
+      <c r="AO196" s="59">
+        <v>0</v>
+      </c>
       <c r="AP196" s="58">
         <f>Q196*AC196/1000000000</f>
         <v>0</v>
@@ -42666,31 +43480,81 @@
       <c r="N197" s="58"/>
       <c r="O197" s="58"/>
       <c r="P197" s="58"/>
-      <c r="Q197" s="58"/>
-      <c r="R197" s="58"/>
-      <c r="S197" s="58"/>
-      <c r="T197" s="58"/>
-      <c r="U197" s="58"/>
-      <c r="V197" s="58"/>
-      <c r="W197" s="58"/>
-      <c r="X197" s="58"/>
-      <c r="Y197" s="58"/>
-      <c r="Z197" s="58"/>
-      <c r="AA197" s="58"/>
-      <c r="AB197" s="58"/>
-      <c r="AC197" s="52"/>
-      <c r="AD197" s="59"/>
-      <c r="AE197" s="59"/>
-      <c r="AF197" s="59"/>
-      <c r="AG197" s="59"/>
-      <c r="AH197" s="59"/>
-      <c r="AI197" s="59"/>
-      <c r="AJ197" s="59"/>
-      <c r="AK197" s="59"/>
-      <c r="AL197" s="59"/>
-      <c r="AM197" s="59"/>
-      <c r="AN197" s="59"/>
-      <c r="AO197" s="59"/>
+      <c r="Q197" s="58">
+        <v>1</v>
+      </c>
+      <c r="R197" s="58">
+        <v>1.1</v>
+      </c>
+      <c r="S197" s="58">
+        <v>1.2</v>
+      </c>
+      <c r="T197" s="58">
+        <v>1.3</v>
+      </c>
+      <c r="U197" s="58">
+        <v>0</v>
+      </c>
+      <c r="V197" s="58">
+        <v>0</v>
+      </c>
+      <c r="W197" s="58">
+        <v>1.6</v>
+      </c>
+      <c r="X197" s="58">
+        <v>1.7</v>
+      </c>
+      <c r="Y197" s="58">
+        <v>0</v>
+      </c>
+      <c r="Z197" s="58">
+        <v>0</v>
+      </c>
+      <c r="AA197" s="58">
+        <v>0</v>
+      </c>
+      <c r="AB197" s="58">
+        <v>0</v>
+      </c>
+      <c r="AC197" s="52">
+        <v>0</v>
+      </c>
+      <c r="AD197" s="59">
+        <v>0</v>
+      </c>
+      <c r="AE197" s="59">
+        <v>0</v>
+      </c>
+      <c r="AF197" s="59">
+        <v>0</v>
+      </c>
+      <c r="AG197" s="59">
+        <v>0</v>
+      </c>
+      <c r="AH197" s="59">
+        <v>0</v>
+      </c>
+      <c r="AI197" s="59">
+        <v>0</v>
+      </c>
+      <c r="AJ197" s="59">
+        <v>0</v>
+      </c>
+      <c r="AK197" s="59">
+        <v>0</v>
+      </c>
+      <c r="AL197" s="59">
+        <v>0</v>
+      </c>
+      <c r="AM197" s="59">
+        <v>0</v>
+      </c>
+      <c r="AN197" s="59">
+        <v>0</v>
+      </c>
+      <c r="AO197" s="59">
+        <v>0</v>
+      </c>
       <c r="AP197" s="58">
         <f>Q197*AC197/1000000000</f>
         <v>0</v>
@@ -42850,31 +43714,81 @@
       <c r="N198" s="58"/>
       <c r="O198" s="58"/>
       <c r="P198" s="58"/>
-      <c r="Q198" s="58"/>
-      <c r="R198" s="58"/>
-      <c r="S198" s="58"/>
-      <c r="T198" s="58"/>
-      <c r="U198" s="58"/>
-      <c r="V198" s="58"/>
-      <c r="W198" s="58"/>
-      <c r="X198" s="58"/>
-      <c r="Y198" s="58"/>
-      <c r="Z198" s="58"/>
-      <c r="AA198" s="58"/>
-      <c r="AB198" s="58"/>
-      <c r="AC198" s="52"/>
-      <c r="AD198" s="59"/>
-      <c r="AE198" s="59"/>
-      <c r="AF198" s="59"/>
-      <c r="AG198" s="59"/>
-      <c r="AH198" s="59"/>
-      <c r="AI198" s="59"/>
-      <c r="AJ198" s="59"/>
-      <c r="AK198" s="59"/>
-      <c r="AL198" s="59"/>
-      <c r="AM198" s="59"/>
-      <c r="AN198" s="59"/>
-      <c r="AO198" s="59"/>
+      <c r="Q198" s="58">
+        <v>17.9</v>
+      </c>
+      <c r="R198" s="58">
+        <v>21.8</v>
+      </c>
+      <c r="S198" s="58">
+        <v>26.5</v>
+      </c>
+      <c r="T198" s="58">
+        <v>42.7</v>
+      </c>
+      <c r="U198" s="58">
+        <v>0</v>
+      </c>
+      <c r="V198" s="58">
+        <v>0</v>
+      </c>
+      <c r="W198" s="58">
+        <v>69.7</v>
+      </c>
+      <c r="X198" s="58">
+        <v>86</v>
+      </c>
+      <c r="Y198" s="58">
+        <v>0</v>
+      </c>
+      <c r="Z198" s="58">
+        <v>0</v>
+      </c>
+      <c r="AA198" s="58">
+        <v>0</v>
+      </c>
+      <c r="AB198" s="58">
+        <v>0</v>
+      </c>
+      <c r="AC198" s="52">
+        <v>0</v>
+      </c>
+      <c r="AD198" s="59">
+        <v>0</v>
+      </c>
+      <c r="AE198" s="59">
+        <v>0</v>
+      </c>
+      <c r="AF198" s="59">
+        <v>0</v>
+      </c>
+      <c r="AG198" s="59">
+        <v>0</v>
+      </c>
+      <c r="AH198" s="59">
+        <v>0</v>
+      </c>
+      <c r="AI198" s="59">
+        <v>0</v>
+      </c>
+      <c r="AJ198" s="59">
+        <v>0</v>
+      </c>
+      <c r="AK198" s="59">
+        <v>0</v>
+      </c>
+      <c r="AL198" s="59">
+        <v>0</v>
+      </c>
+      <c r="AM198" s="59">
+        <v>0</v>
+      </c>
+      <c r="AN198" s="59">
+        <v>0</v>
+      </c>
+      <c r="AO198" s="59">
+        <v>0</v>
+      </c>
       <c r="AP198" s="58">
         <f>Q198*AC198/1000000000</f>
         <v>0</v>
@@ -43034,31 +43948,81 @@
       <c r="N199" s="58"/>
       <c r="O199" s="58"/>
       <c r="P199" s="58"/>
-      <c r="Q199" s="58"/>
-      <c r="R199" s="58"/>
-      <c r="S199" s="58"/>
-      <c r="T199" s="58"/>
-      <c r="U199" s="58"/>
-      <c r="V199" s="58"/>
-      <c r="W199" s="58"/>
-      <c r="X199" s="58"/>
-      <c r="Y199" s="58"/>
-      <c r="Z199" s="58"/>
-      <c r="AA199" s="58"/>
-      <c r="AB199" s="58"/>
-      <c r="AC199" s="52"/>
-      <c r="AD199" s="59"/>
-      <c r="AE199" s="59"/>
-      <c r="AF199" s="59"/>
-      <c r="AG199" s="59"/>
-      <c r="AH199" s="59"/>
-      <c r="AI199" s="59"/>
-      <c r="AJ199" s="59"/>
-      <c r="AK199" s="59"/>
-      <c r="AL199" s="59"/>
-      <c r="AM199" s="59"/>
-      <c r="AN199" s="59"/>
-      <c r="AO199" s="59"/>
+      <c r="Q199" s="58">
+        <v>2.3</v>
+      </c>
+      <c r="R199" s="58">
+        <v>2.5</v>
+      </c>
+      <c r="S199" s="58">
+        <v>2.7</v>
+      </c>
+      <c r="T199" s="58">
+        <v>2.8</v>
+      </c>
+      <c r="U199" s="58">
+        <v>0</v>
+      </c>
+      <c r="V199" s="58">
+        <v>0</v>
+      </c>
+      <c r="W199" s="58">
+        <v>3.3</v>
+      </c>
+      <c r="X199" s="58">
+        <v>3.6</v>
+      </c>
+      <c r="Y199" s="58">
+        <v>0</v>
+      </c>
+      <c r="Z199" s="58">
+        <v>0</v>
+      </c>
+      <c r="AA199" s="58">
+        <v>0</v>
+      </c>
+      <c r="AB199" s="58">
+        <v>0</v>
+      </c>
+      <c r="AC199" s="52">
+        <v>0</v>
+      </c>
+      <c r="AD199" s="59">
+        <v>0</v>
+      </c>
+      <c r="AE199" s="59">
+        <v>0</v>
+      </c>
+      <c r="AF199" s="59">
+        <v>0</v>
+      </c>
+      <c r="AG199" s="59">
+        <v>0</v>
+      </c>
+      <c r="AH199" s="59">
+        <v>0</v>
+      </c>
+      <c r="AI199" s="59">
+        <v>0</v>
+      </c>
+      <c r="AJ199" s="59">
+        <v>0</v>
+      </c>
+      <c r="AK199" s="59">
+        <v>0</v>
+      </c>
+      <c r="AL199" s="59">
+        <v>0</v>
+      </c>
+      <c r="AM199" s="59">
+        <v>0</v>
+      </c>
+      <c r="AN199" s="59">
+        <v>0</v>
+      </c>
+      <c r="AO199" s="59">
+        <v>0</v>
+      </c>
       <c r="AP199" s="58">
         <f>Q199*AC199/1000000000</f>
         <v>0</v>
@@ -43218,31 +44182,81 @@
       <c r="N200" s="58"/>
       <c r="O200" s="58"/>
       <c r="P200" s="58"/>
-      <c r="Q200" s="58"/>
-      <c r="R200" s="58"/>
-      <c r="S200" s="58"/>
-      <c r="T200" s="58"/>
-      <c r="U200" s="58"/>
-      <c r="V200" s="58"/>
-      <c r="W200" s="58"/>
-      <c r="X200" s="58"/>
-      <c r="Y200" s="58"/>
-      <c r="Z200" s="58"/>
-      <c r="AA200" s="58"/>
-      <c r="AB200" s="58"/>
-      <c r="AC200" s="52"/>
-      <c r="AD200" s="59"/>
-      <c r="AE200" s="59"/>
-      <c r="AF200" s="59"/>
-      <c r="AG200" s="59"/>
-      <c r="AH200" s="59"/>
-      <c r="AI200" s="59"/>
-      <c r="AJ200" s="59"/>
-      <c r="AK200" s="59"/>
-      <c r="AL200" s="59"/>
-      <c r="AM200" s="59"/>
-      <c r="AN200" s="59"/>
-      <c r="AO200" s="59"/>
+      <c r="Q200" s="58">
+        <v>76.9</v>
+      </c>
+      <c r="R200" s="58">
+        <v>106.9</v>
+      </c>
+      <c r="S200" s="58">
+        <v>124.1</v>
+      </c>
+      <c r="T200" s="58">
+        <v>107.9</v>
+      </c>
+      <c r="U200" s="58">
+        <v>0</v>
+      </c>
+      <c r="V200" s="58">
+        <v>0</v>
+      </c>
+      <c r="W200" s="58">
+        <v>135.5</v>
+      </c>
+      <c r="X200" s="58">
+        <v>154.1</v>
+      </c>
+      <c r="Y200" s="58">
+        <v>0</v>
+      </c>
+      <c r="Z200" s="58">
+        <v>0</v>
+      </c>
+      <c r="AA200" s="58">
+        <v>0</v>
+      </c>
+      <c r="AB200" s="58">
+        <v>0</v>
+      </c>
+      <c r="AC200" s="52">
+        <v>0</v>
+      </c>
+      <c r="AD200" s="59">
+        <v>0</v>
+      </c>
+      <c r="AE200" s="59">
+        <v>0</v>
+      </c>
+      <c r="AF200" s="59">
+        <v>0</v>
+      </c>
+      <c r="AG200" s="59">
+        <v>0</v>
+      </c>
+      <c r="AH200" s="59">
+        <v>0</v>
+      </c>
+      <c r="AI200" s="59">
+        <v>0</v>
+      </c>
+      <c r="AJ200" s="59">
+        <v>0</v>
+      </c>
+      <c r="AK200" s="59">
+        <v>0</v>
+      </c>
+      <c r="AL200" s="59">
+        <v>0</v>
+      </c>
+      <c r="AM200" s="59">
+        <v>0</v>
+      </c>
+      <c r="AN200" s="59">
+        <v>0</v>
+      </c>
+      <c r="AO200" s="59">
+        <v>0</v>
+      </c>
       <c r="AP200" s="58">
         <f>Q200*AC200/1000000000</f>
         <v>0</v>
@@ -43402,31 +44416,81 @@
       <c r="N201" s="58"/>
       <c r="O201" s="58"/>
       <c r="P201" s="58"/>
-      <c r="Q201" s="58"/>
-      <c r="R201" s="58"/>
-      <c r="S201" s="58"/>
-      <c r="T201" s="58"/>
-      <c r="U201" s="58"/>
-      <c r="V201" s="58"/>
-      <c r="W201" s="58"/>
-      <c r="X201" s="58"/>
-      <c r="Y201" s="58"/>
-      <c r="Z201" s="58"/>
-      <c r="AA201" s="58"/>
-      <c r="AB201" s="58"/>
-      <c r="AC201" s="52"/>
-      <c r="AD201" s="59"/>
-      <c r="AE201" s="59"/>
-      <c r="AF201" s="59"/>
-      <c r="AG201" s="59"/>
-      <c r="AH201" s="59"/>
-      <c r="AI201" s="59"/>
-      <c r="AJ201" s="59"/>
-      <c r="AK201" s="59"/>
-      <c r="AL201" s="59"/>
-      <c r="AM201" s="59"/>
-      <c r="AN201" s="59"/>
-      <c r="AO201" s="59"/>
+      <c r="Q201" s="58">
+        <v>16.3</v>
+      </c>
+      <c r="R201" s="58">
+        <v>5</v>
+      </c>
+      <c r="S201" s="58">
+        <v>5.9</v>
+      </c>
+      <c r="T201" s="58">
+        <v>3.4</v>
+      </c>
+      <c r="U201" s="58">
+        <v>0</v>
+      </c>
+      <c r="V201" s="58">
+        <v>0</v>
+      </c>
+      <c r="W201" s="58">
+        <v>4.5</v>
+      </c>
+      <c r="X201" s="58">
+        <v>5</v>
+      </c>
+      <c r="Y201" s="58">
+        <v>0</v>
+      </c>
+      <c r="Z201" s="58">
+        <v>0</v>
+      </c>
+      <c r="AA201" s="58">
+        <v>0</v>
+      </c>
+      <c r="AB201" s="58">
+        <v>0</v>
+      </c>
+      <c r="AC201" s="52">
+        <v>0</v>
+      </c>
+      <c r="AD201" s="59">
+        <v>0</v>
+      </c>
+      <c r="AE201" s="59">
+        <v>0</v>
+      </c>
+      <c r="AF201" s="59">
+        <v>0</v>
+      </c>
+      <c r="AG201" s="59">
+        <v>0</v>
+      </c>
+      <c r="AH201" s="59">
+        <v>0</v>
+      </c>
+      <c r="AI201" s="59">
+        <v>0</v>
+      </c>
+      <c r="AJ201" s="59">
+        <v>0</v>
+      </c>
+      <c r="AK201" s="59">
+        <v>0</v>
+      </c>
+      <c r="AL201" s="59">
+        <v>0</v>
+      </c>
+      <c r="AM201" s="59">
+        <v>0</v>
+      </c>
+      <c r="AN201" s="59">
+        <v>0</v>
+      </c>
+      <c r="AO201" s="59">
+        <v>0</v>
+      </c>
       <c r="AP201" s="58">
         <f>Q201*AC201/1000000000</f>
         <v>0</v>
@@ -43586,31 +44650,81 @@
       <c r="N202" s="58"/>
       <c r="O202" s="58"/>
       <c r="P202" s="58"/>
-      <c r="Q202" s="58"/>
-      <c r="R202" s="58"/>
-      <c r="S202" s="58"/>
-      <c r="T202" s="58"/>
-      <c r="U202" s="58"/>
-      <c r="V202" s="58"/>
-      <c r="W202" s="58"/>
-      <c r="X202" s="58"/>
-      <c r="Y202" s="58"/>
-      <c r="Z202" s="58"/>
-      <c r="AA202" s="58"/>
-      <c r="AB202" s="58"/>
-      <c r="AC202" s="52"/>
-      <c r="AD202" s="59"/>
-      <c r="AE202" s="59"/>
-      <c r="AF202" s="59"/>
-      <c r="AG202" s="59"/>
-      <c r="AH202" s="59"/>
-      <c r="AI202" s="59"/>
-      <c r="AJ202" s="59"/>
-      <c r="AK202" s="59"/>
-      <c r="AL202" s="59"/>
-      <c r="AM202" s="59"/>
-      <c r="AN202" s="59"/>
-      <c r="AO202" s="59"/>
+      <c r="Q202" s="58">
+        <v>10.5</v>
+      </c>
+      <c r="R202" s="58">
+        <v>11.6</v>
+      </c>
+      <c r="S202" s="58">
+        <v>12.7</v>
+      </c>
+      <c r="T202" s="58">
+        <v>15.6</v>
+      </c>
+      <c r="U202" s="58">
+        <v>0</v>
+      </c>
+      <c r="V202" s="58">
+        <v>0</v>
+      </c>
+      <c r="W202" s="58">
+        <v>20</v>
+      </c>
+      <c r="X202" s="58">
+        <v>22.1</v>
+      </c>
+      <c r="Y202" s="58">
+        <v>0</v>
+      </c>
+      <c r="Z202" s="58">
+        <v>0</v>
+      </c>
+      <c r="AA202" s="58">
+        <v>0</v>
+      </c>
+      <c r="AB202" s="58">
+        <v>0</v>
+      </c>
+      <c r="AC202" s="52">
+        <v>0</v>
+      </c>
+      <c r="AD202" s="59">
+        <v>0</v>
+      </c>
+      <c r="AE202" s="59">
+        <v>0</v>
+      </c>
+      <c r="AF202" s="59">
+        <v>0</v>
+      </c>
+      <c r="AG202" s="59">
+        <v>0</v>
+      </c>
+      <c r="AH202" s="59">
+        <v>0</v>
+      </c>
+      <c r="AI202" s="59">
+        <v>0</v>
+      </c>
+      <c r="AJ202" s="59">
+        <v>0</v>
+      </c>
+      <c r="AK202" s="59">
+        <v>0</v>
+      </c>
+      <c r="AL202" s="59">
+        <v>0</v>
+      </c>
+      <c r="AM202" s="59">
+        <v>0</v>
+      </c>
+      <c r="AN202" s="59">
+        <v>0</v>
+      </c>
+      <c r="AO202" s="59">
+        <v>0</v>
+      </c>
       <c r="AP202" s="58">
         <f>Q202*AC202/1000000000</f>
         <v>0</v>
@@ -43770,31 +44884,81 @@
       <c r="N203" s="58"/>
       <c r="O203" s="58"/>
       <c r="P203" s="58"/>
-      <c r="Q203" s="58"/>
-      <c r="R203" s="58"/>
-      <c r="S203" s="58"/>
-      <c r="T203" s="58"/>
-      <c r="U203" s="58"/>
-      <c r="V203" s="58"/>
-      <c r="W203" s="58"/>
-      <c r="X203" s="58"/>
-      <c r="Y203" s="58"/>
-      <c r="Z203" s="58"/>
-      <c r="AA203" s="58"/>
-      <c r="AB203" s="58"/>
-      <c r="AC203" s="52"/>
-      <c r="AD203" s="59"/>
-      <c r="AE203" s="59"/>
-      <c r="AF203" s="59"/>
-      <c r="AG203" s="59"/>
-      <c r="AH203" s="59"/>
-      <c r="AI203" s="59"/>
-      <c r="AJ203" s="59"/>
-      <c r="AK203" s="59"/>
-      <c r="AL203" s="59"/>
-      <c r="AM203" s="59"/>
-      <c r="AN203" s="59"/>
-      <c r="AO203" s="59"/>
+      <c r="Q203" s="58">
+        <v>68.6</v>
+      </c>
+      <c r="R203" s="58">
+        <v>63.1</v>
+      </c>
+      <c r="S203" s="58">
+        <v>72.4</v>
+      </c>
+      <c r="T203" s="58">
+        <v>77.2</v>
+      </c>
+      <c r="U203" s="58">
+        <v>0</v>
+      </c>
+      <c r="V203" s="58">
+        <v>0</v>
+      </c>
+      <c r="W203" s="58">
+        <v>88.2</v>
+      </c>
+      <c r="X203" s="58">
+        <v>91.4</v>
+      </c>
+      <c r="Y203" s="58">
+        <v>0</v>
+      </c>
+      <c r="Z203" s="58">
+        <v>0</v>
+      </c>
+      <c r="AA203" s="58">
+        <v>0</v>
+      </c>
+      <c r="AB203" s="58">
+        <v>0</v>
+      </c>
+      <c r="AC203" s="52">
+        <v>0</v>
+      </c>
+      <c r="AD203" s="59">
+        <v>0</v>
+      </c>
+      <c r="AE203" s="59">
+        <v>0</v>
+      </c>
+      <c r="AF203" s="59">
+        <v>0</v>
+      </c>
+      <c r="AG203" s="59">
+        <v>0</v>
+      </c>
+      <c r="AH203" s="59">
+        <v>0</v>
+      </c>
+      <c r="AI203" s="59">
+        <v>0</v>
+      </c>
+      <c r="AJ203" s="59">
+        <v>0</v>
+      </c>
+      <c r="AK203" s="59">
+        <v>0</v>
+      </c>
+      <c r="AL203" s="59">
+        <v>0</v>
+      </c>
+      <c r="AM203" s="59">
+        <v>0</v>
+      </c>
+      <c r="AN203" s="59">
+        <v>0</v>
+      </c>
+      <c r="AO203" s="59">
+        <v>0</v>
+      </c>
       <c r="AP203" s="58">
         <f>Q203*AC203/1000000000</f>
         <v>0</v>
@@ -43954,31 +45118,81 @@
       <c r="N204" s="58"/>
       <c r="O204" s="58"/>
       <c r="P204" s="58"/>
-      <c r="Q204" s="58"/>
-      <c r="R204" s="58"/>
-      <c r="S204" s="58"/>
-      <c r="T204" s="58"/>
-      <c r="U204" s="58"/>
-      <c r="V204" s="58"/>
-      <c r="W204" s="58"/>
-      <c r="X204" s="58"/>
-      <c r="Y204" s="58"/>
-      <c r="Z204" s="58"/>
-      <c r="AA204" s="58"/>
-      <c r="AB204" s="58"/>
-      <c r="AC204" s="52"/>
-      <c r="AD204" s="59"/>
-      <c r="AE204" s="59"/>
-      <c r="AF204" s="59"/>
-      <c r="AG204" s="59"/>
-      <c r="AH204" s="59"/>
-      <c r="AI204" s="59"/>
-      <c r="AJ204" s="59"/>
-      <c r="AK204" s="59"/>
-      <c r="AL204" s="59"/>
-      <c r="AM204" s="59"/>
-      <c r="AN204" s="59"/>
-      <c r="AO204" s="59"/>
+      <c r="Q204" s="58">
+        <v>2.8</v>
+      </c>
+      <c r="R204" s="58">
+        <v>3.1</v>
+      </c>
+      <c r="S204" s="58">
+        <v>3.5</v>
+      </c>
+      <c r="T204" s="58">
+        <v>2.9</v>
+      </c>
+      <c r="U204" s="58">
+        <v>0</v>
+      </c>
+      <c r="V204" s="58">
+        <v>0</v>
+      </c>
+      <c r="W204" s="58">
+        <v>3.5</v>
+      </c>
+      <c r="X204" s="58">
+        <v>3.7</v>
+      </c>
+      <c r="Y204" s="58">
+        <v>0</v>
+      </c>
+      <c r="Z204" s="58">
+        <v>0</v>
+      </c>
+      <c r="AA204" s="58">
+        <v>0</v>
+      </c>
+      <c r="AB204" s="58">
+        <v>0</v>
+      </c>
+      <c r="AC204" s="52">
+        <v>0</v>
+      </c>
+      <c r="AD204" s="59">
+        <v>0</v>
+      </c>
+      <c r="AE204" s="59">
+        <v>0</v>
+      </c>
+      <c r="AF204" s="59">
+        <v>0</v>
+      </c>
+      <c r="AG204" s="59">
+        <v>0</v>
+      </c>
+      <c r="AH204" s="59">
+        <v>0</v>
+      </c>
+      <c r="AI204" s="59">
+        <v>0</v>
+      </c>
+      <c r="AJ204" s="59">
+        <v>0</v>
+      </c>
+      <c r="AK204" s="59">
+        <v>0</v>
+      </c>
+      <c r="AL204" s="59">
+        <v>0</v>
+      </c>
+      <c r="AM204" s="59">
+        <v>0</v>
+      </c>
+      <c r="AN204" s="59">
+        <v>0</v>
+      </c>
+      <c r="AO204" s="59">
+        <v>0</v>
+      </c>
       <c r="AP204" s="58">
         <f>Q204*AC204/1000000000</f>
         <v>0</v>
@@ -44138,31 +45352,81 @@
       <c r="N205" s="58"/>
       <c r="O205" s="58"/>
       <c r="P205" s="58"/>
-      <c r="Q205" s="58"/>
-      <c r="R205" s="58"/>
-      <c r="S205" s="58"/>
-      <c r="T205" s="58"/>
-      <c r="U205" s="58"/>
-      <c r="V205" s="58"/>
-      <c r="W205" s="58"/>
-      <c r="X205" s="58"/>
-      <c r="Y205" s="58"/>
-      <c r="Z205" s="58"/>
-      <c r="AA205" s="58"/>
-      <c r="AB205" s="58"/>
-      <c r="AC205" s="52"/>
-      <c r="AD205" s="59"/>
-      <c r="AE205" s="59"/>
-      <c r="AF205" s="59"/>
-      <c r="AG205" s="59"/>
-      <c r="AH205" s="59"/>
-      <c r="AI205" s="59"/>
-      <c r="AJ205" s="59"/>
-      <c r="AK205" s="59"/>
-      <c r="AL205" s="59"/>
-      <c r="AM205" s="59"/>
-      <c r="AN205" s="59"/>
-      <c r="AO205" s="59"/>
+      <c r="Q205" s="58">
+        <v>4</v>
+      </c>
+      <c r="R205" s="58">
+        <v>3.8</v>
+      </c>
+      <c r="S205" s="58">
+        <v>5.3</v>
+      </c>
+      <c r="T205" s="58">
+        <v>0.6</v>
+      </c>
+      <c r="U205" s="58">
+        <v>0</v>
+      </c>
+      <c r="V205" s="58">
+        <v>0</v>
+      </c>
+      <c r="W205" s="58">
+        <v>5.5</v>
+      </c>
+      <c r="X205" s="58">
+        <v>5.7</v>
+      </c>
+      <c r="Y205" s="58">
+        <v>0</v>
+      </c>
+      <c r="Z205" s="58">
+        <v>0</v>
+      </c>
+      <c r="AA205" s="58">
+        <v>0</v>
+      </c>
+      <c r="AB205" s="58">
+        <v>0</v>
+      </c>
+      <c r="AC205" s="52">
+        <v>0</v>
+      </c>
+      <c r="AD205" s="59">
+        <v>0</v>
+      </c>
+      <c r="AE205" s="59">
+        <v>0</v>
+      </c>
+      <c r="AF205" s="59">
+        <v>0</v>
+      </c>
+      <c r="AG205" s="59">
+        <v>0</v>
+      </c>
+      <c r="AH205" s="59">
+        <v>0</v>
+      </c>
+      <c r="AI205" s="59">
+        <v>0</v>
+      </c>
+      <c r="AJ205" s="59">
+        <v>0</v>
+      </c>
+      <c r="AK205" s="59">
+        <v>0</v>
+      </c>
+      <c r="AL205" s="59">
+        <v>0</v>
+      </c>
+      <c r="AM205" s="59">
+        <v>0</v>
+      </c>
+      <c r="AN205" s="59">
+        <v>0</v>
+      </c>
+      <c r="AO205" s="59">
+        <v>0</v>
+      </c>
       <c r="AP205" s="58">
         <f>Q205*AC205/1000000000</f>
         <v>0</v>

</xml_diff>